<commit_message>
update root_id in configuration
</commit_message>
<xml_diff>
--- a/baocao/baocao.xlsx
+++ b/baocao/baocao.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290118" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306726" uniqueCount="397">
   <si>
     <t>CXD</t>
   </si>
@@ -1240,6 +1240,18 @@
   <si>
     <t>3540.000000</t>
   </si>
+  <si>
+    <t>6181</t>
+  </si>
+  <si>
+    <t>6035</t>
+  </si>
+  <si>
+    <t>1842</t>
+  </si>
+  <si>
+    <t>4193</t>
+  </si>
 </sst>
 </file>
 
@@ -2541,76 +2553,76 @@
       <c r="J7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Y7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="Z7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AB7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AC7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AE7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AF7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AG7" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AH7" t="s" s="11">
         <v>27</v>
       </c>
     </row>
@@ -2621,76 +2633,76 @@
       <c r="J8" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="11">
         <v>96</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="11">
         <v>97</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" t="s" s="11">
         <v>99</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" t="s" s="11">
         <v>100</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" t="s" s="11">
         <v>101</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" t="s" s="11">
         <v>102</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" t="s" s="11">
         <v>94</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="X8" t="s">
+      <c r="X8" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Y8" t="s" s="11">
         <v>96</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="Z8" t="s" s="11">
         <v>97</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AB8" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AC8" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AD8" t="s" s="11">
         <v>99</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AE8" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AF8" t="s" s="11">
         <v>100</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AG8" t="s" s="11">
         <v>101</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AH8" t="s" s="11">
         <v>102</v>
       </c>
     </row>
@@ -2762,7 +2774,7 @@
         <v>294</v>
       </c>
       <c r="X9" t="s" s="11">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="Y9" t="s" s="11">
         <v>294</v>
@@ -2878,7 +2890,7 @@
         <v>294</v>
       </c>
       <c r="X10" t="s" s="11">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="Y10" t="s" s="11">
         <v>294</v>
@@ -3574,7 +3586,7 @@
         <v>294</v>
       </c>
       <c r="X16" t="s" s="11">
-        <v>294</v>
+        <v>394</v>
       </c>
       <c r="Y16" t="s" s="11">
         <v>294</v>
@@ -3690,7 +3702,7 @@
         <v>294</v>
       </c>
       <c r="X17" t="s" s="11">
-        <v>294</v>
+        <v>395</v>
       </c>
       <c r="Y17" t="s" s="11">
         <v>294</v>
@@ -3922,7 +3934,7 @@
         <v>294</v>
       </c>
       <c r="X19" t="s" s="11">
-        <v>294</v>
+        <v>396</v>
       </c>
       <c r="Y19" t="s" s="11">
         <v>294</v>
@@ -4325,76 +4337,76 @@
       <c r="J24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="S24" t="s">
+      <c r="S24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="T24" t="s">
+      <c r="T24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" t="s" s="11">
         <v>26</v>
       </c>
-      <c r="V24" t="s">
+      <c r="V24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="X24" t="s">
+      <c r="X24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Y24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="Z24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AA24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AB24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AC24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AD24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AE24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AF24" t="s">
+      <c r="AF24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AG24" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AH24" t="s" s="11">
         <v>27</v>
       </c>
     </row>
@@ -4405,76 +4417,76 @@
       <c r="J25" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" t="s" s="11">
         <v>96</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" t="s" s="11">
         <v>97</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" t="s" s="11">
         <v>99</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S25" t="s" s="11">
         <v>100</v>
       </c>
-      <c r="T25" t="s">
+      <c r="T25" t="s" s="11">
         <v>101</v>
       </c>
-      <c r="U25" t="s">
+      <c r="U25" t="s" s="11">
         <v>102</v>
       </c>
-      <c r="V25" t="s">
+      <c r="V25" t="s" s="11">
         <v>94</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="X25" t="s">
+      <c r="X25" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Y25" t="s" s="11">
         <v>96</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="Z25" t="s" s="11">
         <v>97</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AA25" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AB25" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="AC25" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AD25" t="s" s="11">
         <v>99</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AE25" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AF25" t="s" s="11">
         <v>100</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AG25" t="s" s="11">
         <v>101</v>
       </c>
-      <c r="AH25" t="s">
+      <c r="AH25" t="s" s="11">
         <v>102</v>
       </c>
     </row>
@@ -11580,10 +11592,10 @@
         <v>109</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15" s="27" t="n">
-        <v>99999.0</v>
+        <v>154888.0</v>
       </c>
       <c r="I15" s="27" t="n">
         <v>244870.0</v>
@@ -11592,7 +11604,7 @@
         <v>1302506.0</v>
       </c>
       <c r="K15" s="27" t="n">
-        <v>1647375.0</v>
+        <v>1702264.0</v>
       </c>
       <c r="L15" s="27" t="n">
         <v>0.0</v>
@@ -11658,10 +11670,10 @@
         <v>109</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H16" s="27" t="n">
-        <v>154888.0</v>
+        <v>99999.0</v>
       </c>
       <c r="I16" s="27" t="n">
         <v>244870.0</v>
@@ -11670,7 +11682,7 @@
         <v>1302506.0</v>
       </c>
       <c r="K16" s="27" t="n">
-        <v>1702264.0</v>
+        <v>1647375.0</v>
       </c>
       <c r="L16" s="27" t="n">
         <v>0.0</v>

</xml_diff>